<commit_message>
Added graphs and results
</commit_message>
<xml_diff>
--- a/results/summary_graph_classification_GIN_brf.csv.xlsx
+++ b/results/summary_graph_classification_GIN_brf.csv.xlsx
@@ -1,43 +1,81 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>test_mean</t>
+  </si>
+  <si>
+    <t>test_ci</t>
+  </si>
+  <si>
+    <t>brf_batch_add</t>
+  </si>
+  <si>
+    <t>brf_batch_remove</t>
+  </si>
+  <si>
+    <t>dataset</t>
+  </si>
+  <si>
+    <t>num_iterations</t>
+  </si>
+  <si>
+    <t>enzymes</t>
+  </si>
+  <si>
+    <t>imdb</t>
+  </si>
+  <si>
+    <t>mutag</t>
+  </si>
+  <si>
+    <t>proteins</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -46,30 +84,18 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -77,83 +103,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -441,226 +400,200 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>dataset</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>num_iterations</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>test_mean</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>test_ci</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>brf_batch_add</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>brf_batch_remove</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>enzymes</t>
-        </is>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>42.5</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>0.0418462795372672</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>5</v>
       </c>
-      <c r="F2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n"/>
-      <c r="B3" s="1" t="n">
+      <c r="F2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>42.5</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>0.036040101122068</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>4</v>
       </c>
-      <c r="F3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>imdb</t>
-        </is>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="n">
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4">
         <v>75.40000000000001</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>0.0558891760540446</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>5</v>
       </c>
-      <c r="F4" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n"/>
-      <c r="B5" s="1" t="n">
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1">
         <v>2</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>71.7</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>0.0544095579838689</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5">
         <v>4</v>
       </c>
-      <c r="F5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>mutag</t>
-        </is>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="n">
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6">
         <v>87.5</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>0.1357939615741436</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
         <v>5</v>
       </c>
-      <c r="F6" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n"/>
-      <c r="B7" s="1" t="n">
+      <c r="F6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1">
         <v>2</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>85.50000000000001</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>0.1289961239727768</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
         <v>5</v>
       </c>
-      <c r="F7" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n"/>
-      <c r="B8" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="C8" t="n">
+      <c r="F7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="C8">
         <v>86.49999999999999</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8">
         <v>0.1299615327702778</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8">
         <v>4</v>
       </c>
-      <c r="F8" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>proteins</t>
-        </is>
-      </c>
-      <c r="B9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" t="n">
+      <c r="F8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9">
         <v>75.26785714285712</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9">
         <v>0.0338061701891406</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9">
         <v>5</v>
       </c>
-      <c r="F9" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n"/>
-      <c r="B10" s="1" t="n">
+      <c r="F9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1">
         <v>2</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10">
         <v>75.08928571428571</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10">
         <v>0.0230350221379958</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10">
         <v>4</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F10">
         <v>1</v>
       </c>
     </row>
@@ -671,6 +604,6 @@
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A10"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Experiments with 100 seeds
</commit_message>
<xml_diff>
--- a/results/summary_graph_classification_GIN_brf.csv.xlsx
+++ b/results/summary_graph_classification_GIN_brf.csv.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,16 +496,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>19.66666666666666</v>
+        <v>35.5</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0225092573548455</v>
+        <v>0.0298328677803526</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -514,10 +514,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>30.66666666666667</v>
+        <v>35.66666666666667</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0571936282387392</v>
+        <v>0.0469515116310907</v>
       </c>
       <c r="E3" t="n">
         <v>4</v>
@@ -527,22 +527,18 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>imdb</t>
-        </is>
-      </c>
+      <c r="A4" s="1" t="n"/>
       <c r="B4" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>66.10000000000001</v>
+        <v>35.83333333333334</v>
       </c>
       <c r="D4" t="n">
-        <v>0.04394997155858</v>
+        <v>0.027588242262078</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
@@ -551,20 +547,20 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>mutag</t>
+          <t>imdb</t>
         </is>
       </c>
       <c r="B5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>77</v>
+        <v>72.89999999999999</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0586515131944607</v>
+        <v>0.0244049175372505</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
         <v>2</v>
@@ -576,44 +572,158 @@
         <v>2</v>
       </c>
       <c r="C6" t="n">
-        <v>64.5</v>
+        <v>70.7</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1090412765882718</v>
+        <v>0.0194010309004444</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" s="1" t="n"/>
+      <c r="B7" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" t="n">
+        <v>72</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0375233260785874</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>mutag</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>82.99999999999999</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.08390470785361211</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n"/>
+      <c r="B9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="n">
+        <v>81.5</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0490917508345343</v>
+      </c>
+      <c r="E9" t="n">
+        <v>5</v>
+      </c>
+      <c r="F9" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n"/>
+      <c r="B10" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C10" t="n">
+        <v>76.5</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.0548634668973808</v>
+      </c>
+      <c r="E10" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
         <is>
           <t>proteins</t>
         </is>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B11" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C7" t="n">
-        <v>59.91071428571429</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.0197964772170222</v>
-      </c>
-      <c r="E7" t="n">
-        <v>3</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
+      <c r="C11" t="n">
+        <v>70.98214285714286</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.0247757802241278</v>
+      </c>
+      <c r="E11" t="n">
+        <v>5</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n"/>
+      <c r="B12" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" t="n">
+        <v>72.58928571428571</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.0236969062821908</v>
+      </c>
+      <c r="E12" t="n">
+        <v>4</v>
+      </c>
+      <c r="F12" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n"/>
+      <c r="B13" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" t="n">
+        <v>72.14285714285714</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.0225594452819339</v>
+      </c>
+      <c r="E13" t="n">
+        <v>5</v>
+      </c>
+      <c r="F13" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A5:A6"/>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A13"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>